<commit_message>
Made a new file with all traits
</commit_message>
<xml_diff>
--- a/data/Leptin.xlsx
+++ b/data/Leptin.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FC95CC-C33B-4591-BB3E-1E2ADE9A6722}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2087E8DA-E71C-4D1E-9760-E3DEEDDAABE3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="165">
   <si>
     <t>Paper_ID</t>
   </si>
@@ -471,9 +471,6 @@
   </si>
   <si>
     <t>f-f-fm</t>
-  </si>
-  <si>
-    <t>Assuming 3 months (90 days) from: "GTT and ITT tests were performed in all experimental groups at 3 months of age"</t>
   </si>
   <si>
     <t>NCF2 (Control) HFF2(Treatment)</t>
@@ -1071,31 +1068,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C40BE8-1B59-4041-9B74-03EB3774E13A}">
-  <dimension ref="A1:AU13"/>
+  <dimension ref="A1:AP13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="T1" sqref="T1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:Z13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" style="3" customWidth="1"/>
-    <col min="3" max="8" width="9.140625" style="3"/>
-    <col min="9" max="9" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="21" width="9.140625" style="3"/>
-    <col min="22" max="22" width="16.140625" style="30" customWidth="1"/>
-    <col min="23" max="23" width="16.140625" style="3" customWidth="1"/>
-    <col min="24" max="28" width="9.140625" style="3"/>
-    <col min="29" max="29" width="16.140625" style="3" customWidth="1"/>
-    <col min="30" max="30" width="9.140625" style="3"/>
-    <col min="31" max="31" width="41" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="9.140625" style="3"/>
+    <col min="3" max="7" width="9.140625" style="3"/>
+    <col min="8" max="8" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="17" width="9.140625" style="3"/>
+    <col min="18" max="18" width="16.140625" style="30" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" style="3" customWidth="1"/>
+    <col min="20" max="23" width="9.140625" style="3"/>
+    <col min="24" max="24" width="16.140625" style="3" customWidth="1"/>
+    <col min="25" max="25" width="9.140625" style="3"/>
+    <col min="26" max="26" width="41" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1112,88 +1109,73 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>40</v>
+        <v>129</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>10</v>
+        <v>126</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>129</v>
+        <v>61</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>126</v>
+        <v>62</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>60</v>
+      <c r="R1" s="23" t="s">
+        <v>13</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
-      <c r="V1" s="23" t="s">
-        <v>13</v>
+      <c r="V1" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AF1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
@@ -1209,75 +1191,75 @@
       <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K2" s="2">
+      <c r="J2" s="2">
         <f>12*7</f>
         <v>84</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="R2" s="4">
+      <c r="O2" s="4">
         <v>10.4</v>
       </c>
-      <c r="S2" s="4">
+      <c r="P2" s="4">
         <f>1.5*SQRT(7)</f>
         <v>3.9686269665968861</v>
       </c>
-      <c r="T2" s="4">
-        <f>S2/SQRT(7)</f>
+      <c r="Q2" s="4">
+        <f>P2/SQRT(7)</f>
         <v>1.5</v>
       </c>
-      <c r="V2" s="24">
+      <c r="R2" s="24">
         <v>7</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="X2" s="2">
+      <c r="T2" s="2">
         <v>13.1</v>
       </c>
-      <c r="Y2" s="2">
-        <f>Z2*SQRT(AB2)</f>
+      <c r="U2" s="2">
+        <f>V2*SQRT(W2)</f>
         <v>4.2332020977033453</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="V2" s="2">
         <v>1.6</v>
       </c>
-      <c r="AB2" s="2">
+      <c r="W2" s="2">
         <v>7</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
@@ -1293,73 +1275,73 @@
       <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="2">
+      <c r="J3" s="2">
         <v>84</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="R3" s="4">
+      <c r="O3" s="4">
         <v>10.4</v>
       </c>
-      <c r="S3" s="4">
-        <f t="shared" ref="S3:S5" si="0">1.5*SQRT(7)</f>
+      <c r="P3" s="4">
+        <f t="shared" ref="P3" si="0">1.5*SQRT(7)</f>
         <v>3.9686269665968861</v>
       </c>
-      <c r="T3" s="4">
+      <c r="Q3" s="4">
         <v>1.5</v>
       </c>
-      <c r="V3" s="24">
+      <c r="R3" s="24">
         <v>7</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="X3" s="2">
+      <c r="T3" s="2">
         <v>6.7</v>
       </c>
-      <c r="Y3" s="2">
-        <f t="shared" ref="Y3:Y5" si="1">Z3*SQRT(AB3)</f>
+      <c r="U3" s="2">
+        <f>V3*SQRT(W3)</f>
         <v>2.6457513110645907</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="V3" s="2">
         <v>1</v>
       </c>
-      <c r="AB3" s="2">
+      <c r="W3" s="2">
         <v>7</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AD3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="AE3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -1375,74 +1357,74 @@
       <c r="E4" s="2">
         <v>2</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="2">
+      <c r="J4" s="2">
         <f>12*7</f>
         <v>84</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="R4" s="4">
+      <c r="O4" s="4">
         <v>8.8000000000000007</v>
       </c>
-      <c r="S4" s="4">
+      <c r="P4" s="4">
         <f>1*SQRT(7)</f>
         <v>2.6457513110645907</v>
       </c>
-      <c r="T4" s="4">
+      <c r="Q4" s="4">
         <v>1</v>
       </c>
-      <c r="V4" s="24">
+      <c r="R4" s="24">
         <v>18</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="X4" s="2">
+      <c r="T4" s="2">
         <v>16.3</v>
       </c>
-      <c r="Y4" s="2">
-        <f t="shared" si="1"/>
+      <c r="U4" s="2">
+        <f>V4*SQRT(W4)</f>
         <v>6.3639610306789276</v>
       </c>
-      <c r="Z4" s="2">
+      <c r="V4" s="2">
         <v>1.5</v>
       </c>
-      <c r="AB4" s="2">
+      <c r="W4" s="2">
         <v>18</v>
       </c>
-      <c r="AC4" s="2" t="s">
+      <c r="X4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AD4" s="2" t="s">
+      <c r="Y4" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="AE4" s="2" t="s">
+      <c r="Z4" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -1458,73 +1440,73 @@
       <c r="E5" s="2">
         <v>2</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="2">
+      <c r="J5" s="2">
         <v>84</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="R5" s="4">
+      <c r="O5" s="4">
         <v>8.8000100000000003</v>
       </c>
-      <c r="S5" s="4">
+      <c r="P5" s="4">
         <f>1*SQRT(7)</f>
         <v>2.6457513110645907</v>
       </c>
-      <c r="T5" s="4">
+      <c r="Q5" s="4">
         <v>1</v>
       </c>
-      <c r="V5" s="24">
+      <c r="R5" s="24">
         <v>18</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="S5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="X5" s="2">
+      <c r="T5" s="2">
         <v>8.8000000000000007</v>
       </c>
-      <c r="Y5" s="2">
-        <f t="shared" si="1"/>
+      <c r="U5" s="2">
+        <f>V5*SQRT(W5)</f>
         <v>5.0911688245431419</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="V5" s="2">
         <v>1.2</v>
       </c>
-      <c r="AB5" s="2">
+      <c r="W5" s="2">
         <v>18</v>
       </c>
-      <c r="AC5" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AD5" s="2" t="s">
+      <c r="Y5" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="AE5" s="2" t="s">
+      <c r="Z5" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:47" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>132</v>
       </c>
@@ -1540,69 +1522,69 @@
       <c r="E6" s="8">
         <v>1</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="H6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="8">
+      <c r="J6" s="8">
         <v>270</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="K6" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="L6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="M6" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="Q6" s="8" t="s">
+      <c r="N6" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="R6" s="8">
+      <c r="O6" s="8">
         <v>2.39</v>
       </c>
-      <c r="S6" s="8">
+      <c r="P6" s="8">
         <v>3.87</v>
       </c>
-      <c r="T6" s="8">
+      <c r="Q6" s="8">
         <v>1.29</v>
       </c>
-      <c r="V6" s="25">
+      <c r="R6" s="25">
         <v>9</v>
       </c>
-      <c r="W6" s="8" t="s">
+      <c r="S6" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="X6" s="8">
+      <c r="T6" s="8">
         <v>107.85</v>
       </c>
-      <c r="Y6" s="8">
+      <c r="U6" s="8">
         <v>17.670000000000002</v>
       </c>
-      <c r="Z6" s="8">
+      <c r="V6" s="8">
         <v>5.89</v>
       </c>
-      <c r="AB6" s="8">
+      <c r="W6" s="8">
         <v>9</v>
       </c>
-      <c r="AC6" s="8" t="s">
+      <c r="X6" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AD6" s="8" t="s">
+      <c r="Y6" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="AE6" s="8" t="s">
+      <c r="Z6" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="AU6" s="9"/>
-    </row>
-    <row r="7" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AP6" s="9"/>
+    </row>
+    <row r="7" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>142</v>
       </c>
@@ -1618,76 +1600,76 @@
       <c r="E7" s="10">
         <v>1</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="I7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="K7" s="10">
+      <c r="J7" s="10">
         <v>90</v>
       </c>
-      <c r="N7" s="10" t="s">
+      <c r="K7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="10" t="s">
+      <c r="L7" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="P7" s="11" t="s">
+      <c r="M7" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="Q7" s="12" t="s">
+      <c r="N7" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="R7" s="11">
+      <c r="O7" s="11">
         <v>0.64700000000000002</v>
       </c>
-      <c r="S7" s="10">
+      <c r="P7" s="10">
         <f>0.03*SQRT(5)</f>
         <v>6.7082039324993695E-2</v>
       </c>
-      <c r="T7" s="10">
+      <c r="Q7" s="10">
         <v>0.03</v>
       </c>
-      <c r="V7" s="26">
+      <c r="R7" s="26">
         <v>5</v>
       </c>
-      <c r="W7" s="10" t="s">
+      <c r="S7" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="X7" s="10">
+      <c r="T7" s="10">
         <v>0.83</v>
       </c>
-      <c r="Y7" s="10">
+      <c r="U7" s="10">
         <f>0.04*SQRT(5)</f>
         <v>8.9442719099991588E-2</v>
       </c>
-      <c r="Z7" s="10">
+      <c r="V7" s="10">
         <v>0.04</v>
       </c>
-      <c r="AB7" s="10">
+      <c r="W7" s="10">
         <v>5</v>
       </c>
-      <c r="AC7" s="10" t="s">
+      <c r="X7" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="AD7" s="10" t="s">
+      <c r="Y7" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="AE7" s="10" t="s">
+      <c r="Z7" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="AF7" s="10" t="s">
-        <v>150</v>
+      <c r="AA7" s="10" t="s">
+        <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:47" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>145</v>
       </c>
@@ -1703,492 +1685,485 @@
       <c r="E8" s="13">
         <v>1</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="F8" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="G8" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="H8" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="I8" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="K8" s="13">
+      <c r="J8" s="13">
         <v>90</v>
       </c>
+      <c r="K8" s="13" t="s">
+        <v>30</v>
+      </c>
       <c r="L8" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="O8" s="15">
+        <v>1.19</v>
+      </c>
+      <c r="P8" s="13">
+        <v>1.2</v>
+      </c>
+      <c r="Q8" s="13">
+        <f>P7/SQRT(9)</f>
+        <v>2.2360679774997897E-2</v>
+      </c>
+      <c r="R8" s="27">
+        <v>9</v>
+      </c>
+      <c r="S8" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="T8" s="15">
+        <v>63.8</v>
+      </c>
+      <c r="U8" s="15">
+        <v>3.8</v>
+      </c>
+      <c r="V8" s="13">
+        <f>U8/SQRT(9)</f>
+        <v>1.2666666666666666</v>
+      </c>
+      <c r="W8" s="13">
+        <v>9</v>
+      </c>
+      <c r="X8" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y8" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z8" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="N8" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="O8" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="P8" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q8" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="R8" s="15">
-        <v>1.19</v>
-      </c>
-      <c r="S8" s="13">
-        <v>1.2</v>
-      </c>
-      <c r="T8" s="13">
-        <f>S7/SQRT(9)</f>
-        <v>2.2360679774997897E-2</v>
-      </c>
-      <c r="V8" s="27">
-        <v>9</v>
-      </c>
-      <c r="W8" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="X8" s="15">
-        <v>63.8</v>
-      </c>
-      <c r="Y8" s="15">
-        <v>3.8</v>
-      </c>
-      <c r="Z8" s="13">
-        <f>Y8/SQRT(9)</f>
-        <v>1.2666666666666666</v>
-      </c>
-      <c r="AB8" s="13">
-        <v>9</v>
-      </c>
-      <c r="AC8" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="AD8" s="13" t="s">
+    </row>
+    <row r="9" spans="1:42" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="AE8" s="13" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="9" spans="1:47" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="B9" s="17" t="s">
         <v>152</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>153</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>134</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E9" s="16">
         <v>1</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="F9" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="G9" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="H9" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="I9" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="K9" s="16">
+      <c r="J9" s="16">
         <f>12*7</f>
         <v>84</v>
       </c>
-      <c r="N9" s="16" t="s">
+      <c r="K9" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="O9" s="16" t="s">
+      <c r="L9" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="P9" s="18" t="s">
+      <c r="M9" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="Q9" s="18" t="s">
+      <c r="N9" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="R9" s="18">
+      <c r="O9" s="18">
         <v>0.229896907216495</v>
       </c>
-      <c r="S9" s="18">
+      <c r="P9" s="18">
         <v>0.10713716335477599</v>
       </c>
-      <c r="T9" s="18">
+      <c r="Q9" s="18">
         <v>3.0927835051546403E-2</v>
       </c>
-      <c r="U9" s="18"/>
-      <c r="V9" s="28">
+      <c r="R9" s="28">
         <v>12</v>
       </c>
-      <c r="W9" s="18" t="s">
+      <c r="S9" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="X9" s="18">
+      <c r="T9" s="18">
         <v>0.54742268041237097</v>
       </c>
-      <c r="Y9" s="18">
+      <c r="U9" s="18">
         <v>0.27855662472241699</v>
       </c>
-      <c r="Z9" s="18">
+      <c r="V9" s="18">
         <v>8.0412371134020597E-2</v>
       </c>
-      <c r="AB9" s="16">
+      <c r="W9" s="16">
         <v>12</v>
       </c>
-      <c r="AC9" s="18" t="s">
+      <c r="X9" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="AD9" s="16" t="s">
+      <c r="Y9" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z9" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA9" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="AE9" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="AF9" s="16" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="1:47" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:42" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>134</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E10" s="16">
         <v>2</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="F10" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="G10" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="H10" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="I10" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="K10" s="16">
+      <c r="J10" s="16">
         <f>24*7</f>
         <v>168</v>
       </c>
-      <c r="N10" s="16" t="s">
+      <c r="K10" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="O10" s="16" t="s">
+      <c r="L10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="P10" s="18" t="s">
+      <c r="M10" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="Q10" s="18" t="s">
+      <c r="N10" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="R10" s="18">
+      <c r="O10" s="18">
         <v>0.20927835051546398</v>
       </c>
-      <c r="S10" s="18">
+      <c r="P10" s="18">
         <v>7.8567253126835906E-2</v>
       </c>
-      <c r="T10" s="18">
+      <c r="Q10" s="18">
         <v>2.26804123711341E-2</v>
       </c>
-      <c r="U10" s="18"/>
-      <c r="V10" s="28">
+      <c r="R10" s="28">
         <v>12</v>
       </c>
-      <c r="W10" s="18" t="s">
+      <c r="S10" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="X10" s="18">
+      <c r="T10" s="18">
         <v>0.56597938144329907</v>
       </c>
-      <c r="Y10" s="18">
+      <c r="U10" s="18">
         <v>0.24998671449447699</v>
       </c>
-      <c r="Z10" s="18">
+      <c r="V10" s="18">
         <v>7.2164948453608102E-2</v>
       </c>
-      <c r="AB10" s="16">
+      <c r="W10" s="16">
         <v>12</v>
       </c>
-      <c r="AC10" s="18" t="s">
+      <c r="X10" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="AD10" s="16" t="s">
-        <v>159</v>
+      <c r="Y10" s="16" t="s">
+        <v>158</v>
       </c>
-      <c r="AE10" s="16" t="s">
+      <c r="Z10" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA10" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="AF10" s="16" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="11" spans="1:47" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:42" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>134</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E11" s="16">
         <v>1</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="F11" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="G11" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="H11" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="I11" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="K11" s="16">
+      <c r="J11" s="16">
         <v>84</v>
       </c>
-      <c r="N11" s="16" t="s">
+      <c r="K11" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="O11" s="16" t="s">
+      <c r="L11" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="P11" s="18" t="s">
+      <c r="M11" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="Q11" s="18" t="s">
+      <c r="N11" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="R11" s="18">
+      <c r="O11" s="18">
         <v>0.229896907216495</v>
       </c>
-      <c r="S11" s="18">
+      <c r="P11" s="18">
         <v>0.10713716335477599</v>
       </c>
-      <c r="T11" s="18">
+      <c r="Q11" s="18">
         <v>3.0927835051546403E-2</v>
       </c>
-      <c r="U11" s="18"/>
-      <c r="V11" s="28">
+      <c r="R11" s="28">
         <v>12</v>
       </c>
-      <c r="W11" s="18" t="s">
+      <c r="S11" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="X11" s="18">
+      <c r="T11" s="18">
         <v>0.31030927835051503</v>
       </c>
-      <c r="Y11" s="18">
+      <c r="U11" s="18">
         <v>0.135707073582716</v>
       </c>
-      <c r="Z11" s="18">
+      <c r="V11" s="18">
         <v>3.91752577319587E-2</v>
       </c>
-      <c r="AB11" s="16">
+      <c r="W11" s="16">
         <v>12</v>
       </c>
-      <c r="AC11" s="18" t="s">
+      <c r="X11" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="AD11" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="AE11" s="16" t="s">
+      <c r="Y11" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="AF11" s="16" t="s">
-        <v>156</v>
+      <c r="Z11" s="16" t="s">
+        <v>157</v>
       </c>
-    </row>
-    <row r="12" spans="1:47" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AA11" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>134</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E12" s="16">
         <v>2</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="F12" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="G12" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="H12" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="I12" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="K12" s="16">
+      <c r="J12" s="16">
         <v>168</v>
       </c>
-      <c r="N12" s="16" t="s">
+      <c r="K12" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="O12" s="16" t="s">
+      <c r="L12" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="P12" s="18" t="s">
+      <c r="M12" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="Q12" s="18" t="s">
+      <c r="N12" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="R12" s="18">
+      <c r="O12" s="18">
         <v>0.20927835051546398</v>
       </c>
-      <c r="S12" s="18">
+      <c r="P12" s="18">
         <v>7.8567253126835906E-2</v>
       </c>
-      <c r="T12" s="18">
+      <c r="Q12" s="18">
         <v>2.26804123711341E-2</v>
       </c>
-      <c r="U12" s="18"/>
-      <c r="V12" s="28">
+      <c r="R12" s="28">
         <v>12</v>
       </c>
-      <c r="W12" s="18" t="s">
+      <c r="S12" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="X12" s="18">
+      <c r="T12" s="18">
         <v>0.33092783505154599</v>
       </c>
-      <c r="Y12" s="18">
+      <c r="U12" s="18">
         <v>0.135707073582716</v>
       </c>
-      <c r="Z12" s="18">
+      <c r="V12" s="18">
         <v>3.9175257731958804E-2</v>
       </c>
-      <c r="AB12" s="16">
+      <c r="W12" s="16">
         <v>12</v>
       </c>
-      <c r="AC12" s="18" t="s">
+      <c r="X12" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="AD12" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="AE12" s="16" t="s">
+      <c r="Y12" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="AF12" s="16" t="s">
-        <v>156</v>
+      <c r="Z12" s="16" t="s">
+        <v>157</v>
       </c>
-    </row>
-    <row r="13" spans="1:47" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AA12" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E13" s="19">
         <v>1</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="F13" s="19" t="s">
         <v>35</v>
       </c>
+      <c r="G13" s="19" t="s">
+        <v>162</v>
+      </c>
       <c r="H13" s="19" t="s">
-        <v>163</v>
+        <v>31</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="K13" s="21">
+      <c r="J13" s="21">
         <f>12*7</f>
         <v>84</v>
       </c>
-      <c r="N13" s="19" t="s">
+      <c r="K13" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="O13" s="19" t="s">
+      <c r="L13" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="P13" s="22" t="s">
+      <c r="M13" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="Q13" s="22" t="s">
+      <c r="N13" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="R13" s="22">
+      <c r="O13" s="22">
         <v>22.195119999999999</v>
       </c>
-      <c r="S13" s="22">
+      <c r="P13" s="22">
         <v>1.349753</v>
       </c>
-      <c r="T13" s="22">
+      <c r="Q13" s="22">
         <v>0.42682930000000002</v>
       </c>
-      <c r="V13" s="29">
+      <c r="R13" s="29">
         <v>10</v>
       </c>
-      <c r="W13" s="22" t="s">
+      <c r="S13" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="X13" s="22">
+      <c r="T13" s="22">
         <v>29.7561</v>
       </c>
-      <c r="Y13" s="22">
+      <c r="U13" s="22">
         <v>2.3138619999999999</v>
       </c>
-      <c r="Z13" s="22">
+      <c r="V13" s="22">
         <v>0.73170729999999995</v>
       </c>
-      <c r="AB13" s="29">
+      <c r="W13" s="29">
         <v>10</v>
       </c>
-      <c r="AC13" s="22" t="s">
+      <c r="X13" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="AD13" s="19" t="s">
-        <v>165</v>
+      <c r="Y13" s="19" t="s">
+        <v>164</v>
       </c>
-      <c r="AE13" s="19" t="s">
-        <v>164</v>
+      <c r="Z13" s="19" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>